<commit_message>
añadir algun caso mas en el ejercicio-3
</commit_message>
<xml_diff>
--- a/ejercicios-QA-manual/Ejercicio-3 Pack de Regresión RAUL FABRA.xlsx
+++ b/ejercicios-QA-manual/Ejercicio-3 Pack de Regresión RAUL FABRA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holacons\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holacons\Desktop\EJERCICIOS QA MANUAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F17D6595-24C9-41E5-92A5-C21C657F64B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B45FCF8-3A55-40AF-BD35-5BDB8A7AA514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D792FA8-DF88-4463-B710-B07C2870B1D3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -205,6 +205,24 @@
   </si>
   <si>
     <t xml:space="preserve">Visualizar el desglose del precio Final con descuento aplicado </t>
+  </si>
+  <si>
+    <t>VY-IBE-010</t>
+  </si>
+  <si>
+    <t>Validar la reserva de los vuelos de iberia</t>
+  </si>
+  <si>
+    <t>VY-IBE-011</t>
+  </si>
+  <si>
+    <t>Validar los pagos de la reserva de los vuelos Iberia</t>
+  </si>
+  <si>
+    <t>"seria seguir los pasos de la pagina de reservas"</t>
+  </si>
+  <si>
+    <t>"Seria seguir los pasos de introducir los datos de la tarjeta bancaria"</t>
   </si>
 </sst>
 </file>
@@ -525,33 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -559,15 +550,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -592,27 +574,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -629,10 +598,61 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -951,7 +971,7 @@
   <dimension ref="B1:N80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,15 +987,15 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -984,13 +1004,13 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -999,13 +1019,13 @@
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -1051,7 +1071,7 @@
       <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -1071,1025 +1091,1001 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="46"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="23"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="2:14" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="48"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="24"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="2:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="49"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="37" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="41"/>
-      <c r="I11" s="25"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="2:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="49"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="30" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="25"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="50"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="26"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="46"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="36" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="23"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="2:14" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="48"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="24"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="49"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="30" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="25"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="38"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="50"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39" t="s">
+      <c r="B18" s="33"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="26"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="39"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="46"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="36" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="23"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" spans="2:9" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="40" t="s">
+      <c r="H20" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="48"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="36" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="40"/>
-      <c r="I21" s="24"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="41"/>
     </row>
     <row r="22" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="49"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="30" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="25"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="50"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="26"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="46"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="36" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="27"/>
-      <c r="I24" s="23"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" spans="2:9" s="11" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="40" t="s">
+      <c r="H25" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="I25" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="48"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="36" t="s">
+      <c r="B26" s="31"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="40"/>
-      <c r="I26" s="24"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="49"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="30" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="41"/>
-      <c r="I27" s="25"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="38"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="50"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39" t="s">
+      <c r="B28" s="33"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="26"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="39"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="46"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="36" t="s">
+      <c r="B29" s="29"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="27"/>
-      <c r="I29" s="23"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="14"/>
     </row>
     <row r="30" spans="2:9" s="11" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="36" t="s">
+      <c r="F30" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="40" t="s">
+      <c r="H30" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I30" s="24" t="s">
+      <c r="I30" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="48"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="36" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="29" t="s">
+      <c r="G31" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="40"/>
-      <c r="I31" s="24"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="49"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="30" t="s">
+      <c r="B32" s="32"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="41"/>
-      <c r="I32" s="25"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="38"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="50"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39" t="s">
+      <c r="B33" s="33"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H33" s="42"/>
-      <c r="I33" s="26"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="39"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="46"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="36" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="27"/>
-      <c r="I34" s="23"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="14"/>
     </row>
     <row r="35" spans="2:9" s="11" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="36" t="s">
+      <c r="F35" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G35" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="40" t="s">
+      <c r="H35" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="24" t="s">
+      <c r="I35" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="48"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="36" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="24"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="41"/>
     </row>
     <row r="37" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="49"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="30" t="s">
+      <c r="B37" s="32"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="41"/>
-      <c r="I37" s="25"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="38"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="50"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39" t="s">
+      <c r="B38" s="33"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H38" s="42"/>
-      <c r="I38" s="26"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="39"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="46"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="36" t="s">
+      <c r="B39" s="29"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="27"/>
-      <c r="I39" s="23"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="14"/>
     </row>
     <row r="40" spans="2:9" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="44" t="s">
+      <c r="E40" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F40" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="36" t="s">
+      <c r="G40" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="40" t="s">
+      <c r="H40" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I40" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="48"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="36" t="s">
+      <c r="B41" s="31"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="G41" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H41" s="40"/>
-      <c r="I41" s="24"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="41"/>
     </row>
     <row r="42" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="49"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="30" t="s">
+      <c r="B42" s="32"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="41"/>
-      <c r="I42" s="25"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="38"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="50"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39" t="s">
+      <c r="B43" s="33"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H43" s="42"/>
-      <c r="I43" s="26"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="39"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="46"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="36" t="s">
+      <c r="B44" s="29"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H44" s="27"/>
-      <c r="I44" s="23"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="14"/>
     </row>
     <row r="45" spans="2:9" s="11" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="44" t="s">
+      <c r="E45" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G45" s="36" t="s">
+      <c r="G45" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="52" t="s">
+      <c r="H45" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="I45" s="24" t="s">
+      <c r="I45" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="48"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29" t="s">
+      <c r="B46" s="31"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="52"/>
-      <c r="I46" s="24"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
     </row>
     <row r="47" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="49"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="30" t="s">
+      <c r="B47" s="32"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H47" s="41"/>
-      <c r="I47" s="25"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="38"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="50"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39" t="s">
+      <c r="B48" s="33"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H48" s="42"/>
-      <c r="I48" s="26"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="39"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="46"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="36" t="s">
+      <c r="B49" s="29"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H49" s="27"/>
-      <c r="I49" s="23"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="14"/>
     </row>
     <row r="50" spans="2:9" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="36" t="s">
+      <c r="F50" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="36" t="s">
+      <c r="G50" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="40" t="s">
+      <c r="H50" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="I50" s="24" t="s">
+      <c r="I50" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="48"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29" t="s">
+      <c r="B51" s="31"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H51" s="40"/>
-      <c r="I51" s="24"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="41"/>
     </row>
     <row r="52" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="49"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="37" t="s">
+      <c r="B52" s="32"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G52" s="30" t="s">
+      <c r="G52" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H52" s="41"/>
-      <c r="I52" s="25"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="38"/>
     </row>
     <row r="53" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="49"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="30" t="s">
+      <c r="B53" s="32"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
     </row>
     <row r="54" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="49"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="30" t="s">
+      <c r="B54" s="32"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="50"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="39" t="s">
+      <c r="B55" s="33"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="46"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="23"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="14"/>
     </row>
     <row r="57" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="47"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="52"/>
-      <c r="I57" s="24"/>
+      <c r="B57" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="41" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B58" s="48"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="24"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="41"/>
     </row>
     <row r="59" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="49"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="25"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="38"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B60" s="50"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="26"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="39"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B61" s="46"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="23"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="14"/>
     </row>
     <row r="62" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="47"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="24"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B63" s="48"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="24"/>
+      <c r="B62" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B63" s="31"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="17"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="41"/>
     </row>
     <row r="64" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="49"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="25"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="38"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B65" s="50"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="26"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="39"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B66" s="46"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="23"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="14"/>
     </row>
     <row r="67" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="47"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="52"/>
-      <c r="I67" s="24"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="40"/>
+      <c r="I67" s="41"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B68" s="48"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="52"/>
-      <c r="I68" s="24"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="40"/>
+      <c r="I68" s="41"/>
     </row>
     <row r="69" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="49"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="41"/>
-      <c r="I69" s="25"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="38"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B70" s="50"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="26"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="39"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B71" s="46"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="23"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="14"/>
     </row>
     <row r="72" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="47"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="24"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="40"/>
+      <c r="I72" s="41"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B73" s="48"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="24"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="40"/>
+      <c r="I73" s="41"/>
     </row>
     <row r="74" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="49"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="41"/>
-      <c r="I74" s="25"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="38"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B75" s="50"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="42"/>
-      <c r="I75" s="26"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="39"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B76" s="46"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="23"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="14"/>
     </row>
     <row r="77" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="47"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="52"/>
-      <c r="I77" s="24"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="40"/>
+      <c r="I77" s="41"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B78" s="48"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="34"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="52"/>
-      <c r="I78" s="24"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="40"/>
+      <c r="I78" s="41"/>
     </row>
     <row r="79" spans="2:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="49"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="30"/>
-      <c r="H79" s="41"/>
-      <c r="I79" s="25"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="36"/>
+      <c r="I79" s="38"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B80" s="50"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="31"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="26"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="H74:H75"/>
-    <mergeCell ref="I74:I75"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="I77:I78"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="I67:I68"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="H72:H73"/>
-    <mergeCell ref="I72:I73"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="H52:H55"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="H17:H18"/>
@@ -2099,6 +2095,54 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="I11:I13"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="I67:I68"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="H72:H73"/>
+    <mergeCell ref="I72:I73"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="I79:I80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>